<commit_message>
ICT TA March 25,2020
</commit_message>
<xml_diff>
--- a/_fmlReport.xlsx
+++ b/_fmlReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>OFFICE</t>
   </si>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">OFFICEPERIOD: </t>
   </si>
   <si>
-    <t>Month of March 2020</t>
+    <t>Month of February 2020</t>
   </si>
   <si>
     <t>No.</t>
@@ -84,25 +84,25 @@
     <t>Time</t>
   </si>
   <si>
-    <t>2020-00221</t>
-  </si>
-  <si>
-    <t>2020-03-02</t>
-  </si>
-  <si>
-    <t>1:40 PM</t>
-  </si>
-  <si>
-    <t>RESTITUTO BASOY NANEZ, III</t>
-  </si>
-  <si>
-    <t>FAD-RICTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          Cannot print properly                                                                                                 </t>
-  </si>
-  <si>
-    <t>PRINTER/SCANNER</t>
+    <t>2020-00218</t>
+  </si>
+  <si>
+    <t>2020-02-19</t>
+  </si>
+  <si>
+    <t>9:00 AM</t>
+  </si>
+  <si>
+    <t>JOHN CARLO MOJARES HERNANDEZ</t>
+  </si>
+  <si>
+    <t>LGMED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                    Activation Failed and have no internet connection                                                    </t>
+  </si>
+  <si>
+    <t>INTERNET CONNECTIVITY</t>
   </si>
   <si>
     <t>Mark Kim Sacluti</t>
@@ -111,19 +111,19 @@
     <t>2020-03-10</t>
   </si>
   <si>
-    <t>1:41 PM</t>
-  </si>
-  <si>
-    <t>1:47 PM</t>
-  </si>
-  <si>
-    <t>6minutes</t>
-  </si>
-  <si>
-    <t>2020-00220</t>
-  </si>
-  <si>
-    <t>9:16 AM</t>
+    <t>9:10 AM</t>
+  </si>
+  <si>
+    <t>0 hours and 10 minutes</t>
+  </si>
+  <si>
+    <t>2020-00219</t>
+  </si>
+  <si>
+    <t>2020-02-27</t>
+  </si>
+  <si>
+    <t>11:00 AM</t>
   </si>
   <si>
     <t>KRISTOFFER GUINTO MOJICA</t>
@@ -132,8 +132,8 @@
     <t>LGMED-PDMU</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Validation of Subaybayan accounts
+    <t xml:space="preserve">*SUBAYBAYAN Account of Engr. Rom Joseph V. Pineda
+*Accessibility issue
 </t>
   </si>
   <si>
@@ -143,221 +143,35 @@
     <t>Shiela Mei Olivar</t>
   </si>
   <si>
-    <t>9:20 AM</t>
-  </si>
-  <si>
-    <t>9:22 AM</t>
-  </si>
-  <si>
-    <t>2minutes</t>
-  </si>
-  <si>
-    <t>2020-00222</t>
-  </si>
-  <si>
-    <t>2020-03-09</t>
-  </si>
-  <si>
-    <t>10:03 AM</t>
-  </si>
-  <si>
-    <t>ALLAN ABUSTAN SALVATUS</t>
-  </si>
-  <si>
-    <t>LGMED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          MS Office could not be activated.
-                                                                            </t>
-  </si>
-  <si>
-    <t>10:15 AM</t>
-  </si>
-  <si>
-    <t>10:20 AM</t>
-  </si>
-  <si>
-    <t>5minutes</t>
-  </si>
-  <si>
-    <t>2020-00223</t>
-  </si>
-  <si>
-    <t>8:00 AM</t>
-  </si>
-  <si>
-    <t>BEZALEEL ONG SOLTURA</t>
-  </si>
-  <si>
-    <t>FAD-GSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-                                                  </t>
-  </si>
-  <si>
-    <t>INTERNET CONNECTIVITY</t>
-  </si>
-  <si>
-    <t>0000-00-00</t>
-  </si>
-  <si>
-    <t>0minutes</t>
-  </si>
-  <si>
-    <t>2020-00224</t>
-  </si>
-  <si>
-    <t>2:03 PM</t>
-  </si>
-  <si>
-    <t>Rex Oscar L Segunial</t>
-  </si>
-  <si>
-    <t>FAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          Cannot perform print sharing                          </t>
-  </si>
-  <si>
-    <t>2:10 PM</t>
-  </si>
-  <si>
-    <t>2:15 PM</t>
-  </si>
-  <si>
-    <t>2020-00225</t>
-  </si>
-  <si>
-    <t>MARY JANICE BALAHADIA SOBREMONTE</t>
-  </si>
-  <si>
-    <t>LGCDD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cant access LGU account
-                                                 </t>
-  </si>
-  <si>
-    <t>2020-00226</t>
-  </si>
-  <si>
-    <t>4:03 PM</t>
-  </si>
-  <si>
-    <t>JUDY ANN RIVAS SILVA</t>
-  </si>
-  <si>
-    <t>ORD-8888</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          cannot access to the internet
-                                                                            </t>
-  </si>
-  <si>
-    <t>4:05 PM</t>
-  </si>
-  <si>
-    <t>4:10 PM</t>
-  </si>
-  <si>
-    <t>2020-00227</t>
-  </si>
-  <si>
-    <t>LADY CEZANIE  ABEJERO SABANAL</t>
-  </si>
-  <si>
-    <t>ORD-Planning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cannot print properly 
-                                                  </t>
-  </si>
-  <si>
-    <t>2020-00228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No internet connection 
-                                                  </t>
-  </si>
-  <si>
-    <t>2020-00229</t>
-  </si>
-  <si>
-    <t>7:03 AM</t>
-  </si>
-  <si>
-    <t>JORDAN VILLANUEVA NADAL</t>
-  </si>
-  <si>
-    <t>ORD-Legal</t>
+    <t>1:05 PM</t>
+  </si>
+  <si>
+    <t>2 hours and 5 minutes</t>
+  </si>
+  <si>
+    <t>2020-00217</t>
+  </si>
+  <si>
+    <t>2020-02-10</t>
+  </si>
+  <si>
+    <t>10:00 AM</t>
+  </si>
+  <si>
+    <t>LAICA NAREDO MELANIO</t>
+  </si>
+  <si>
+    <t>FAD-Accounting</t>
   </si>
   <si>
     <t xml:space="preserve">                          
-Cannot connect to the internet                          </t>
-  </si>
-  <si>
-    <t>8:15 AM</t>
-  </si>
-  <si>
-    <t>15minutes</t>
-  </si>
-  <si>
-    <t>2020-00230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unable to print through network sharing
-                                                  </t>
-  </si>
-  <si>
-    <t>2020-00231</t>
-  </si>
-  <si>
-    <t>3:03 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LGU P4 account
--Cant upload files and activities 
--no assigned role 
--update City/Municipality            </t>
-  </si>
-  <si>
-    <t>1:00 AM</t>
-  </si>
-  <si>
-    <t>2020-0232</t>
-  </si>
-  <si>
-    <t>2020-03-11</t>
-  </si>
-  <si>
-    <t>MARK KIM ALEJO SACLUTI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample 
-                                                  </t>
-  </si>
-  <si>
-    <t>2020-0233</t>
-  </si>
-  <si>
-    <t>10:57 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          sample problem
-                                                                            </t>
-  </si>
-  <si>
-    <t>DESKTOP/LAPTOP</t>
-  </si>
-  <si>
-    <t>11:03 AM</t>
-  </si>
-  <si>
-    <t>12:18 PM</t>
-  </si>
-  <si>
-    <t>75minutes</t>
+No internet connection                          </t>
+  </si>
+  <si>
+    <t>9:03 AM</t>
+  </si>
+  <si>
+    <t>0 hours and 0 minutes</t>
   </si>
 </sst>
 </file>
@@ -527,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="34">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -616,39 +430,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="6" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
@@ -1061,7 +842,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1262,16 +1043,16 @@
         <v>29</v>
       </c>
       <c r="M15" s="30" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="N15" s="30" t="s">
         <v>29</v>
       </c>
       <c r="O15" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" s="30" t="s">
         <v>31</v>
-      </c>
-      <c r="P15" s="30" t="s">
-        <v>32</v>
       </c>
       <c r="Q15" s="30">
         <v>5</v>
@@ -1282,10 +1063,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>22</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>34</v>
@@ -1308,19 +1089,19 @@
       </c>
       <c r="K16" s="30"/>
       <c r="L16" s="30" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="M16" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="30" t="s">
+      <c r="P16" s="30" t="s">
         <v>41</v>
-      </c>
-      <c r="P16" s="30" t="s">
-        <v>42</v>
       </c>
       <c r="Q16" s="30">
         <v>5</v>
@@ -1331,579 +1112,257 @@
         <v>3</v>
       </c>
       <c r="B17" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="D17" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="E17" s="33" t="s">
         <v>45</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>46</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="30" t="s">
-        <v>48</v>
-      </c>
       <c r="I17" s="30" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>28</v>
       </c>
       <c r="K17" s="30"/>
       <c r="L17" s="30" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="M17" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="P17" s="30" t="s">
         <v>49</v>
-      </c>
-      <c r="N17" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="O17" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="P17" s="30" t="s">
-        <v>51</v>
       </c>
       <c r="Q17" s="30">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:17" customHeight="1" ht="53">
-      <c r="A18" s="30">
-        <v>4</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>54</v>
-      </c>
+    <row r="18" spans="1:17">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="30"/>
-      <c r="G18" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
       <c r="K18" s="30"/>
-      <c r="L18" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M18" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="N18" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O18" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="P18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q18" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" customHeight="1" ht="53">
-      <c r="A19" s="30">
-        <v>5</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>62</v>
-      </c>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="N19" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="O19" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="P19" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q19" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" customHeight="1" ht="53">
-      <c r="A20" s="30">
-        <v>6</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>68</v>
-      </c>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="30"/>
-      <c r="G20" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" s="30" t="s">
-        <v>39</v>
-      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
       <c r="K20" s="30"/>
-      <c r="L20" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M20" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="N20" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O20" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="P20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q20" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" customHeight="1" ht="53">
-      <c r="A21" s="30">
-        <v>7</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>73</v>
-      </c>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="30"/>
-      <c r="G21" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
       <c r="K21" s="30"/>
-      <c r="L21" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="M21" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="N21" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="O21" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="P21" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q21" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" customHeight="1" ht="53">
-      <c r="A22" s="30">
-        <v>8</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>79</v>
-      </c>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="30"/>
-      <c r="G22" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="J22" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
       <c r="K22" s="30"/>
-      <c r="L22" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M22" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="N22" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O22" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="P22" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q22" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" customHeight="1" ht="53">
-      <c r="A23" s="30">
-        <v>9</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>79</v>
-      </c>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="30"/>
-      <c r="G23" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J23" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
       <c r="K23" s="30"/>
-      <c r="L23" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="P23" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q23" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" customHeight="1" ht="53">
-      <c r="A24" s="30">
-        <v>10</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>86</v>
-      </c>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
       <c r="F24" s="30"/>
-      <c r="G24" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J24" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
       <c r="K24" s="30"/>
-      <c r="L24" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="N24" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="P24" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q24" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" customHeight="1" ht="53">
-      <c r="A25" s="30">
-        <v>11</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>62</v>
-      </c>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="30"/>
-      <c r="G25" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>38</v>
-      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
       <c r="J25" s="30"/>
       <c r="K25" s="30"/>
-      <c r="L25" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M25" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="N25" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O25" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="P25" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q25" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" customHeight="1" ht="53">
-      <c r="A26" s="30">
-        <v>12</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>68</v>
-      </c>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="30"/>
-      <c r="G26" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>38</v>
-      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
       <c r="J26" s="30"/>
       <c r="K26" s="30"/>
-      <c r="L26" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="M26" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="N26" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="O26" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="P26" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q26" s="30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" customHeight="1" ht="53">
-      <c r="A27" s="30">
-        <v>13</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="43" t="s">
-        <v>99</v>
-      </c>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="I27" s="30" t="s">
-        <v>38</v>
-      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
-      <c r="L27" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="M27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="O27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="P27" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q27" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" customHeight="1" ht="53">
-      <c r="A28" s="30">
-        <v>14</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>35</v>
-      </c>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
       <c r="F28" s="30"/>
-      <c r="G28" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="J28" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
       <c r="K28" s="30"/>
-      <c r="L28" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="M28" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="N28" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="O28" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="P28" s="30" t="s">
-        <v>107</v>
-      </c>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
       <c r="Q28" s="30"/>
     </row>
     <row r="29" spans="1:17">
@@ -2253,17 +1712,6 @@
     <mergeCell ref="E11:Q11"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
march 26 ict ta
</commit_message>
<xml_diff>
--- a/_fmlReport.xlsx
+++ b/_fmlReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>OFFICE</t>
   </si>
@@ -166,6 +166,9 @@
   <si>
     <t xml:space="preserve">                          
 No internet connection                          </t>
+  </si>
+  <si>
+    <t>Christian Paul Ferrer</t>
   </si>
   <si>
     <t>9:03 AM</t>
@@ -1134,23 +1137,23 @@
         <v>27</v>
       </c>
       <c r="J17" s="30" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="K17" s="30"/>
       <c r="L17" s="30" t="s">
         <v>29</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N17" s="30" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P17" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q17" s="30">
         <v>5</v>

</xml_diff>

<commit_message>
fix dynamic changing of control no
</commit_message>
<xml_diff>
--- a/_fmlReport.xlsx
+++ b/_fmlReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>OFFICE</t>
   </si>
@@ -36,7 +36,7 @@
     <t xml:space="preserve">OFFICEPERIOD: </t>
   </si>
   <si>
-    <t>Month of February 2020</t>
+    <t>Month of May 2020</t>
   </si>
   <si>
     <t>No.</t>
@@ -84,91 +84,55 @@
     <t>Time</t>
   </si>
   <si>
-    <t>2020-00218</t>
-  </si>
-  <si>
-    <t>2020-02-19</t>
-  </si>
-  <si>
-    <t>9:00 AM</t>
-  </si>
-  <si>
-    <t>JOHN CARLO MOJARES HERNANDEZ</t>
-  </si>
-  <si>
-    <t>LGMED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                    Activation Failed and have no internet connection                                                    </t>
-  </si>
-  <si>
-    <t>INTERNET CONNECTIVITY</t>
-  </si>
-  <si>
-    <t>Mark Kim Sacluti</t>
-  </si>
-  <si>
-    <t>2020-03-10</t>
-  </si>
-  <si>
-    <t>9:10 AM</t>
-  </si>
-  <si>
-    <t>0 hours and 10 minutes</t>
-  </si>
-  <si>
-    <t>2020-00219</t>
-  </si>
-  <si>
-    <t>2020-02-27</t>
-  </si>
-  <si>
-    <t>11:00 AM</t>
-  </si>
-  <si>
-    <t>KRISTOFFER GUINTO MOJICA</t>
-  </si>
-  <si>
-    <t>LGMED-PDMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*SUBAYBAYAN Account of Engr. Rom Joseph V. Pineda
-*Accessibility issue
-</t>
+    <t>2020-243</t>
+  </si>
+  <si>
+    <t>2020-05-08</t>
+  </si>
+  <si>
+    <t>12:35 PM</t>
+  </si>
+  <si>
+    <t>NOEL R BARTOLABAC</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>ddw</t>
+  </si>
+  <si>
+    <t>DESKTOP/LAPTOP</t>
+  </si>
+  <si>
+    <t>Charles Adrian T. Odi</t>
+  </si>
+  <si>
+    <t>1:09 PM</t>
+  </si>
+  <si>
+    <t>4:28 AM</t>
+  </si>
+  <si>
+    <t>12 hours and 9 minutes</t>
+  </si>
+  <si>
+    <t>2020-244</t>
+  </si>
+  <si>
+    <t>2020-05-13</t>
+  </si>
+  <si>
+    <t>9:49 AM</t>
+  </si>
+  <si>
+    <t>test1</t>
   </si>
   <si>
     <t>SOFTWARE/SYSTEM</t>
   </si>
   <si>
-    <t>0000-00-00</t>
-  </si>
-  <si>
-    <t>12:00 AM</t>
-  </si>
-  <si>
     <t>0 hours and 0 minutes</t>
-  </si>
-  <si>
-    <t>2020-00217</t>
-  </si>
-  <si>
-    <t>2020-02-10</t>
-  </si>
-  <si>
-    <t>10:00 AM</t>
-  </si>
-  <si>
-    <t>LAICA NAREDO MELANIO</t>
-  </si>
-  <si>
-    <t>FAD-Accounting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          
-No internet connection                          </t>
-  </si>
-  <si>
-    <t>9:03 AM</t>
   </si>
 </sst>
 </file>
@@ -749,7 +713,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" view="pageLayout" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -947,14 +911,12 @@
       </c>
       <c r="K15" s="21"/>
       <c r="L15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="N15" s="21"/>
       <c r="O15" s="21" t="s">
         <v>30</v>
       </c>
@@ -962,7 +924,7 @@
         <v>31</v>
       </c>
       <c r="Q15" s="21">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" customHeight="1" ht="53">
@@ -979,89 +941,53 @@
         <v>34</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="P16" s="21" t="s">
-        <v>41</v>
-      </c>
       <c r="Q16" s="21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" customHeight="1" ht="53">
-      <c r="A17" s="21">
-        <v>3</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="N17" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="P17" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q17" s="21">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="9"/>
@@ -1618,7 +1544,6 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E11:Q11"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>